<commit_message>
cambiar archivos para cargar el nuevo padron
</commit_message>
<xml_diff>
--- a/assets/coordinadores.xlsx
+++ b/assets/coordinadores.xlsx
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>BAJA</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>CHOCOLATE</t>
   </si>
@@ -55,56 +52,20 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="4"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -113,10 +74,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,58 +412,54 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="1">
-        <v>3679</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2">
+        <v>3564</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="1">
-        <v>3680</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3">
+        <v>3565</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="1">
-        <v>3681</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="A4">
+        <v>3566</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="1">
-        <v>3682</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="A5">
+        <v>3567</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="1">
-        <v>3683</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>